<commit_message>
Fixed Test data set for non-intersecting cases
</commit_message>
<xml_diff>
--- a/test_data_set/TEST1.xlsx
+++ b/test_data_set/TEST1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamil\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamil\Desktop\Repozytorium\ComputerGraphics-Toolbox\test_data_set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C6696D-D171-46EF-959C-2DFD6A2B0C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C8563D-E95C-4C60-8054-7A686C8C3D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{015A9D0D-CCA4-48CC-8328-209D941627E7}"/>
   </bookViews>
@@ -66,18 +66,9 @@
     <t>nan</t>
   </si>
   <si>
-    <t>równoległe (w poziomie)</t>
-  </si>
-  <si>
     <t>typ</t>
   </si>
   <si>
-    <t>równoległe (w pionie)</t>
-  </si>
-  <si>
-    <t>równoległe (na ukos)</t>
-  </si>
-  <si>
     <t>na jednej prostej (pion)</t>
   </si>
   <si>
@@ -96,41 +87,57 @@
     <t>na jednej prostej (ukos+0)</t>
   </si>
   <si>
-    <t>równoległe (w poziomie+0)</t>
-  </si>
-  <si>
-    <t>równoległe (w pionie+0)</t>
-  </si>
-  <si>
-    <t>równoległe (na ukos+0)</t>
-  </si>
-  <si>
     <t>takie prawie T</t>
   </si>
   <si>
     <t>takie prawie T (0)</t>
   </si>
   <si>
-    <t>"zwykłe" nieprzecinające się</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>"zwykłe" nieprzecinające się (0)</t>
-  </si>
-  <si>
     <t>Zbiory testowe</t>
+  </si>
+  <si>
+    <t>rownolegle (w poziomie)</t>
+  </si>
+  <si>
+    <t>rownolegle (w poziomie)+0</t>
+  </si>
+  <si>
+    <t>rownolegle (w pionie+0)</t>
+  </si>
+  <si>
+    <t>rownolegle (w pionie)</t>
+  </si>
+  <si>
+    <t>rownolegle (na ukos)</t>
+  </si>
+  <si>
+    <t>rownolegle (na ukos)+0</t>
+  </si>
+  <si>
+    <t>"zwykle" nieprzecinajace sie</t>
+  </si>
+  <si>
+    <t>"zwykle" nieprzecinajace sie+0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -221,10 +228,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -549,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680DB2A7-0E51-4492-93DD-8909CF02A997}">
   <dimension ref="A1:X39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,32 +566,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
+      <c r="A1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -621,7 +628,7 @@
         <v>10</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M2" s="8"/>
     </row>
@@ -660,7 +667,7 @@
         <v>11</v>
       </c>
       <c r="L3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -698,7 +705,7 @@
         <v>11</v>
       </c>
       <c r="L4" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -736,7 +743,7 @@
         <v>11</v>
       </c>
       <c r="L5" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -774,7 +781,7 @@
         <v>11</v>
       </c>
       <c r="L6" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -812,7 +819,7 @@
         <v>11</v>
       </c>
       <c r="L7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -850,7 +857,7 @@
         <v>11</v>
       </c>
       <c r="L8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -888,7 +895,7 @@
         <v>11</v>
       </c>
       <c r="L9" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -926,7 +933,7 @@
         <v>11</v>
       </c>
       <c r="L10" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -964,7 +971,7 @@
         <v>11</v>
       </c>
       <c r="L11" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -1002,7 +1009,7 @@
         <v>11</v>
       </c>
       <c r="L12" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -1040,7 +1047,7 @@
         <v>11</v>
       </c>
       <c r="L13" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -1078,7 +1085,7 @@
         <v>11</v>
       </c>
       <c r="L14" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -1116,7 +1123,7 @@
         <v>11</v>
       </c>
       <c r="L15" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
@@ -1154,7 +1161,7 @@
         <v>11</v>
       </c>
       <c r="L16" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1192,7 +1199,7 @@
         <v>11</v>
       </c>
       <c r="L17" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1230,7 +1237,7 @@
         <v>11</v>
       </c>
       <c r="L18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1268,7 +1275,7 @@
         <v>11</v>
       </c>
       <c r="L19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1306,7 +1313,7 @@
         <v>11</v>
       </c>
       <c r="L20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1344,7 +1351,7 @@
         <v>11</v>
       </c>
       <c r="L21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1382,7 +1389,7 @@
         <v>11</v>
       </c>
       <c r="L22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1420,7 +1427,7 @@
         <v>11</v>
       </c>
       <c r="L23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1458,7 +1465,7 @@
         <v>11</v>
       </c>
       <c r="L24" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1504,7 +1511,7 @@
         <v>11</v>
       </c>
       <c r="L25" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1542,7 +1549,7 @@
         <v>11</v>
       </c>
       <c r="L26" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1580,7 +1587,7 @@
         <v>11</v>
       </c>
       <c r="L27" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1618,7 +1625,7 @@
         <v>11</v>
       </c>
       <c r="L28" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1656,7 +1663,7 @@
         <v>11</v>
       </c>
       <c r="L29" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1694,7 +1701,7 @@
         <v>11</v>
       </c>
       <c r="L30" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -1732,7 +1739,7 @@
         <v>11</v>
       </c>
       <c r="L31" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1770,7 +1777,7 @@
         <v>11</v>
       </c>
       <c r="L32" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -1808,7 +1815,7 @@
         <v>11</v>
       </c>
       <c r="L33" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -1846,7 +1853,7 @@
         <v>11</v>
       </c>
       <c r="L34" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -1884,7 +1891,7 @@
         <v>11</v>
       </c>
       <c r="L35" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -1922,7 +1929,7 @@
         <v>11</v>
       </c>
       <c r="L36" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -1942,7 +1949,7 @@
         <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G37">
         <v>4</v>
@@ -1960,7 +1967,7 @@
         <v>11</v>
       </c>
       <c r="L37" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -1998,7 +2005,7 @@
         <v>11</v>
       </c>
       <c r="L38" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2036,13 +2043,14 @@
         <v>11</v>
       </c>
       <c r="L39" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>